<commit_message>
Experimentos com ambos data sets
</commit_message>
<xml_diff>
--- a/resultados.xlsx
+++ b/resultados.xlsx
@@ -7,7 +7,11 @@
     <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="k=5" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="k=5 e dataset = 0" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="k=10 e dataset = 0" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="k=5 e dataset = 1" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="k=10 e dataset = 1" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -426,6 +430,24 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -476,22 +498,22 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>93.85343890700202</v>
+        <v>94.02887750349323</v>
       </c>
       <c r="C2" t="n">
-        <v>96.67870051452141</v>
+        <v>97.10294117647059</v>
       </c>
       <c r="D2" t="n">
-        <v>0.06109118461608887</v>
+        <v>0.03121280670166016</v>
       </c>
       <c r="E2" t="n">
-        <v>92.97619047619045</v>
+        <v>92.61760596180716</v>
       </c>
       <c r="F2" t="n">
-        <v>95.92766018734456</v>
+        <v>95.45961285428429</v>
       </c>
       <c r="G2" t="n">
-        <v>0.2047438621520996</v>
+        <v>0.06900334358215332</v>
       </c>
     </row>
     <row r="3">
@@ -499,22 +521,22 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>93.49324639031205</v>
+        <v>93.85188635305077</v>
       </c>
       <c r="C3" t="n">
-        <v>96.25347325347326</v>
+        <v>96.72607767455889</v>
       </c>
       <c r="D3" t="n">
-        <v>0.04202961921691895</v>
+        <v>0.03775405883789062</v>
       </c>
       <c r="E3" t="n">
-        <v>93.32080200501252</v>
+        <v>92.62381617761216</v>
       </c>
       <c r="F3" t="n">
-        <v>95.82278496984378</v>
+        <v>95.86228313625736</v>
       </c>
       <c r="G3" t="n">
-        <v>0.1960735321044922</v>
+        <v>0.06249332427978516</v>
       </c>
     </row>
     <row r="4">
@@ -522,22 +544,22 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>94.02421984163949</v>
+        <v>93.67334264865704</v>
       </c>
       <c r="C4" t="n">
-        <v>97.02117467778578</v>
+        <v>96.63307362812222</v>
       </c>
       <c r="D4" t="n">
-        <v>0.04500818252563477</v>
+        <v>0.03775763511657715</v>
       </c>
       <c r="E4" t="n">
-        <v>93.32393483709274</v>
+        <v>92.26672876882472</v>
       </c>
       <c r="F4" t="n">
-        <v>96.37941429775175</v>
+        <v>95.12558949357526</v>
       </c>
       <c r="G4" t="n">
-        <v>0.1709964275360107</v>
+        <v>0.0771794319152832</v>
       </c>
     </row>
     <row r="5">
@@ -545,22 +567,22 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>93.83946592144078</v>
+        <v>94.19655333022823</v>
       </c>
       <c r="C5" t="n">
-        <v>96.96125188079655</v>
+        <v>96.69365079365079</v>
       </c>
       <c r="D5" t="n">
-        <v>0.04484033584594727</v>
+        <v>0.02116727828979492</v>
       </c>
       <c r="E5" t="n">
-        <v>93.1484962406015</v>
+        <v>93.31625523986958</v>
       </c>
       <c r="F5" t="n">
-        <v>96.14399826819125</v>
+        <v>96.03117479970706</v>
       </c>
       <c r="G5" t="n">
-        <v>0.1837515830993652</v>
+        <v>0.07811594009399414</v>
       </c>
     </row>
     <row r="6">
@@ -568,22 +590,22 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>93.67489520260828</v>
+        <v>93.8441235832945</v>
       </c>
       <c r="C6" t="n">
-        <v>96.33425304568058</v>
+        <v>96.4924295774648</v>
       </c>
       <c r="D6" t="n">
-        <v>0.04502773284912109</v>
+        <v>0.02215790748596191</v>
       </c>
       <c r="E6" t="n">
-        <v>92.96992481203009</v>
+        <v>92.79614966620089</v>
       </c>
       <c r="F6" t="n">
-        <v>95.30780231693923</v>
+        <v>96.11186845684351</v>
       </c>
       <c r="G6" t="n">
-        <v>0.1865370273590088</v>
+        <v>0.07811450958251953</v>
       </c>
     </row>
     <row r="7">
@@ -591,22 +613,22 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>93.49014128240955</v>
+        <v>94.20586865393572</v>
       </c>
       <c r="C7" t="n">
-        <v>96.63355542450243</v>
+        <v>96.8404515474468</v>
       </c>
       <c r="D7" t="n">
-        <v>0.04902052879333496</v>
+        <v>0.0377657413482666</v>
       </c>
       <c r="E7" t="n">
-        <v>93.49624060150376</v>
+        <v>92.97469337059464</v>
       </c>
       <c r="F7" t="n">
-        <v>96.30019476804351</v>
+        <v>95.43166908255625</v>
       </c>
       <c r="G7" t="n">
-        <v>0.2114243507385254</v>
+        <v>0.06248164176940918</v>
       </c>
     </row>
     <row r="8">
@@ -614,22 +636,22 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>93.67334264865704</v>
+        <v>94.20742120788699</v>
       </c>
       <c r="C8" t="n">
-        <v>96.202151799687</v>
+        <v>96.90673874390811</v>
       </c>
       <c r="D8" t="n">
-        <v>0.04278802871704102</v>
+        <v>0.02213907241821289</v>
       </c>
       <c r="E8" t="n">
-        <v>92.80075187969923</v>
+        <v>93.67023754075454</v>
       </c>
       <c r="F8" t="n">
-        <v>95.73937900718195</v>
+        <v>96.59835313915124</v>
       </c>
       <c r="G8" t="n">
-        <v>0.1859004497528076</v>
+        <v>0.07810831069946289</v>
       </c>
     </row>
     <row r="9">
@@ -637,22 +659,22 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>94.02887750349326</v>
+        <v>94.19810588417947</v>
       </c>
       <c r="C9" t="n">
-        <v>96.93327466896331</v>
+        <v>96.85026737967914</v>
       </c>
       <c r="D9" t="n">
-        <v>0.04903960227966309</v>
+        <v>0.01562929153442383</v>
       </c>
       <c r="E9" t="n">
-        <v>92.80388471177945</v>
+        <v>92.79149200434715</v>
       </c>
       <c r="F9" t="n">
-        <v>95.810745852466</v>
+        <v>96.10345367064529</v>
       </c>
       <c r="G9" t="n">
-        <v>0.1770942211151123</v>
+        <v>0.08579182624816895</v>
       </c>
     </row>
     <row r="10">
@@ -660,22 +682,22 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>93.6686849868033</v>
+        <v>94.19965843813071</v>
       </c>
       <c r="C10" t="n">
-        <v>96.64793785070242</v>
+        <v>97.2394105347993</v>
       </c>
       <c r="D10" t="n">
-        <v>0.02635049819946289</v>
+        <v>0.02443790435791016</v>
       </c>
       <c r="E10" t="n">
-        <v>92.61278195488721</v>
+        <v>92.97158826269212</v>
       </c>
       <c r="F10" t="n">
-        <v>96.13248455474066</v>
+        <v>95.50383106721135</v>
       </c>
       <c r="G10" t="n">
-        <v>0.1794478893280029</v>
+        <v>0.07349276542663574</v>
       </c>
     </row>
     <row r="11">
@@ -683,22 +705,22 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>94.55053563111319</v>
+        <v>94.19965843813071</v>
       </c>
       <c r="C11" t="n">
-        <v>97.54098637680727</v>
+        <v>96.94532830518537</v>
       </c>
       <c r="D11" t="n">
-        <v>0.07867527008056641</v>
+        <v>0.01563072204589844</v>
       </c>
       <c r="E11" t="n">
-        <v>92.97305764411027</v>
+        <v>93.85033379909953</v>
       </c>
       <c r="F11" t="n">
-        <v>96.28326966439488</v>
+        <v>96.63345098795837</v>
       </c>
       <c r="G11" t="n">
-        <v>0.1850075721740723</v>
+        <v>0.06899118423461914</v>
       </c>
     </row>
     <row r="12">
@@ -706,22 +728,22 @@
         <v>11</v>
       </c>
       <c r="B12" t="n">
-        <v>94.20276354603322</v>
+        <v>94.19965843813071</v>
       </c>
       <c r="C12" t="n">
-        <v>96.91414264770394</v>
+        <v>96.9630413192057</v>
       </c>
       <c r="D12" t="n">
-        <v>0.05899858474731445</v>
+        <v>0.0312495231628418</v>
       </c>
       <c r="E12" t="n">
-        <v>92.97619047619048</v>
+        <v>92.96072038503338</v>
       </c>
       <c r="F12" t="n">
-        <v>96.00119725309477</v>
+        <v>96.56834138910524</v>
       </c>
       <c r="G12" t="n">
-        <v>0.2145872116088867</v>
+        <v>0.08464980125427246</v>
       </c>
     </row>
     <row r="13">
@@ -729,22 +751,22 @@
         <v>12</v>
       </c>
       <c r="B13" t="n">
-        <v>94.02577239559074</v>
+        <v>94.02266728768825</v>
       </c>
       <c r="C13" t="n">
-        <v>96.99268743561456</v>
+        <v>96.93976312377607</v>
       </c>
       <c r="D13" t="n">
-        <v>0.04218196868896484</v>
+        <v>0.03124237060546875</v>
       </c>
       <c r="E13" t="n">
-        <v>93.49937343358394</v>
+        <v>93.14702685918336</v>
       </c>
       <c r="F13" t="n">
-        <v>96.41706287716474</v>
+        <v>96.66033591302133</v>
       </c>
       <c r="G13" t="n">
-        <v>0.1990592479705811</v>
+        <v>0.0690009593963623</v>
       </c>
     </row>
     <row r="14">
@@ -752,22 +774,22 @@
         <v>13</v>
       </c>
       <c r="B14" t="n">
-        <v>94.02887750349323</v>
+        <v>94.19965843813071</v>
       </c>
       <c r="C14" t="n">
-        <v>96.85616230884774</v>
+        <v>96.92097026604068</v>
       </c>
       <c r="D14" t="n">
-        <v>0.04388308525085449</v>
+        <v>0.03124308586120605</v>
       </c>
       <c r="E14" t="n">
-        <v>93.49937343358397</v>
+        <v>92.62071106970969</v>
       </c>
       <c r="F14" t="n">
-        <v>96.16666481776839</v>
+        <v>96.03922578533401</v>
       </c>
       <c r="G14" t="n">
-        <v>0.1815223693847656</v>
+        <v>0.07542729377746582</v>
       </c>
     </row>
     <row r="15">
@@ -775,22 +797,22 @@
         <v>14</v>
       </c>
       <c r="B15" t="n">
-        <v>93.32557056357709</v>
+        <v>94.3766495885732</v>
       </c>
       <c r="C15" t="n">
-        <v>95.8403452952204</v>
+        <v>97.01131243409067</v>
       </c>
       <c r="D15" t="n">
-        <v>0.03704214096069336</v>
+        <v>0.01931023597717285</v>
       </c>
       <c r="E15" t="n">
-        <v>93.1484962406015</v>
+        <v>91.91895668374477</v>
       </c>
       <c r="F15" t="n">
-        <v>95.81145222571369</v>
+        <v>95.28302796795948</v>
       </c>
       <c r="G15" t="n">
-        <v>0.2317118644714355</v>
+        <v>0.07249903678894043</v>
       </c>
     </row>
     <row r="16">
@@ -798,22 +820,22 @@
         <v>15</v>
       </c>
       <c r="B16" t="n">
-        <v>94.37509703462196</v>
+        <v>93.67334264865704</v>
       </c>
       <c r="C16" t="n">
-        <v>97.17227277227278</v>
+        <v>96.51783784124464</v>
       </c>
       <c r="D16" t="n">
-        <v>0.04986667633056641</v>
+        <v>0.03124237060546875</v>
       </c>
       <c r="E16" t="n">
-        <v>93.31766917293234</v>
+        <v>93.49635149821455</v>
       </c>
       <c r="F16" t="n">
-        <v>95.89974937343358</v>
+        <v>96.06424419359271</v>
       </c>
       <c r="G16" t="n">
-        <v>0.2036659717559814</v>
+        <v>0.08462285995483398</v>
       </c>
     </row>
     <row r="17">
@@ -821,22 +843,22 @@
         <v>16</v>
       </c>
       <c r="B17" t="n">
-        <v>93.85499146095327</v>
+        <v>94.03043005744451</v>
       </c>
       <c r="C17" t="n">
-        <v>96.66011801594114</v>
+        <v>96.926339913956</v>
       </c>
       <c r="D17" t="n">
-        <v>0.04753661155700684</v>
+        <v>0.03124165534973145</v>
       </c>
       <c r="E17" t="n">
-        <v>92.96679197994987</v>
+        <v>93.84101847539202</v>
       </c>
       <c r="F17" t="n">
-        <v>96.25621305033071</v>
+        <v>96.39632178578431</v>
       </c>
       <c r="G17" t="n">
-        <v>0.1910660266876221</v>
+        <v>0.06900453567504883</v>
       </c>
     </row>
     <row r="18">
@@ -844,22 +866,22 @@
         <v>17</v>
       </c>
       <c r="B18" t="n">
-        <v>93.14081664337834</v>
+        <v>94.02266728768825</v>
       </c>
       <c r="C18" t="n">
-        <v>95.86040644224788</v>
+        <v>96.99106611078022</v>
       </c>
       <c r="D18" t="n">
-        <v>0.03605222702026367</v>
+        <v>0.03124380111694336</v>
       </c>
       <c r="E18" t="n">
-        <v>93.50250626566415</v>
+        <v>92.96537804688712</v>
       </c>
       <c r="F18" t="n">
-        <v>96.2991881203088</v>
+        <v>95.76675976807451</v>
       </c>
       <c r="G18" t="n">
-        <v>0.1734836101531982</v>
+        <v>0.06899499893188477</v>
       </c>
     </row>
     <row r="19">
@@ -867,22 +889,22 @@
         <v>18</v>
       </c>
       <c r="B19" t="n">
-        <v>93.85343890700202</v>
+        <v>94.3766495885732</v>
       </c>
       <c r="C19" t="n">
-        <v>96.25135909841794</v>
+        <v>97.24029045768177</v>
       </c>
       <c r="D19" t="n">
-        <v>0.03497028350830078</v>
+        <v>0.01562142372131348</v>
       </c>
       <c r="E19" t="n">
-        <v>93.14223057644109</v>
+        <v>93.67179009470578</v>
       </c>
       <c r="F19" t="n">
-        <v>95.99843549762846</v>
+        <v>96.72550860719875</v>
       </c>
       <c r="G19" t="n">
-        <v>0.2115893363952637</v>
+        <v>0.1122581958770752</v>
       </c>
     </row>
     <row r="20">
@@ -890,22 +912,22 @@
         <v>19</v>
       </c>
       <c r="B20" t="n">
-        <v>93.84722869119703</v>
+        <v>93.6655798789008</v>
       </c>
       <c r="C20" t="n">
-        <v>96.58916349838265</v>
+        <v>96.25716625716626</v>
       </c>
       <c r="D20" t="n">
-        <v>0.03191375732421875</v>
+        <v>0.0412604808807373</v>
       </c>
       <c r="E20" t="n">
-        <v>93.48370927318295</v>
+        <v>93.67023754075454</v>
       </c>
       <c r="F20" t="n">
-        <v>96.15338530448886</v>
+        <v>96.42769482391425</v>
       </c>
       <c r="G20" t="n">
-        <v>0.1960723400115967</v>
+        <v>0.1314873695373535</v>
       </c>
     </row>
     <row r="21">
@@ -913,22 +935,22 @@
         <v>20</v>
       </c>
       <c r="B21" t="n">
-        <v>94.03198261139576</v>
+        <v>94.37043937276822</v>
       </c>
       <c r="C21" t="n">
-        <v>97.14500433780744</v>
+        <v>97.12987150149623</v>
       </c>
       <c r="D21" t="n">
-        <v>0.05791306495666504</v>
+        <v>0.03124046325683594</v>
       </c>
       <c r="E21" t="n">
-        <v>93.14536340852131</v>
+        <v>92.61760596180716</v>
       </c>
       <c r="F21" t="n">
-        <v>95.83217157286492</v>
+        <v>95.58476975990006</v>
       </c>
       <c r="G21" t="n">
-        <v>0.1927182674407959</v>
+        <v>0.1515297889709473</v>
       </c>
     </row>
     <row r="22">
@@ -936,22 +958,22 @@
         <v>21</v>
       </c>
       <c r="B22" t="n">
-        <v>93.67179009470578</v>
+        <v>94.02111473373699</v>
       </c>
       <c r="C22" t="n">
-        <v>96.62622743110548</v>
+        <v>96.88573999100315</v>
       </c>
       <c r="D22" t="n">
-        <v>0.03949189186096191</v>
+        <v>0.03124332427978516</v>
       </c>
       <c r="E22" t="n">
-        <v>92.96052631578947</v>
+        <v>92.62071106970969</v>
       </c>
       <c r="F22" t="n">
-        <v>96.04117257871127</v>
+        <v>95.56854031117055</v>
       </c>
       <c r="G22" t="n">
-        <v>0.1774241924285889</v>
+        <v>0.08914995193481445</v>
       </c>
     </row>
     <row r="23">
@@ -959,22 +981,22 @@
         <v>22</v>
       </c>
       <c r="B23" t="n">
-        <v>94.55053563111319</v>
+        <v>93.84412358329453</v>
       </c>
       <c r="C23" t="n">
-        <v>97.51249481112495</v>
+        <v>96.93092414831546</v>
       </c>
       <c r="D23" t="n">
-        <v>0.06355619430541992</v>
+        <v>0.02129077911376953</v>
       </c>
       <c r="E23" t="n">
-        <v>93.31453634085213</v>
+        <v>92.44216736531592</v>
       </c>
       <c r="F23" t="n">
-        <v>95.90328662482364</v>
+        <v>95.47015464662523</v>
       </c>
       <c r="G23" t="n">
-        <v>0.2376291751861572</v>
+        <v>0.06249475479125977</v>
       </c>
     </row>
     <row r="24">
@@ -982,22 +1004,22 @@
         <v>23</v>
       </c>
       <c r="B24" t="n">
-        <v>93.67334264865704</v>
+        <v>94.03198261139576</v>
       </c>
       <c r="C24" t="n">
-        <v>96.60340691300445</v>
+        <v>96.59259868120628</v>
       </c>
       <c r="D24" t="n">
-        <v>0.04250335693359375</v>
+        <v>0.03775334358215332</v>
       </c>
       <c r="E24" t="n">
-        <v>93.31453634085213</v>
+        <v>92.44216736531594</v>
       </c>
       <c r="F24" t="n">
-        <v>95.79192610774683</v>
+        <v>96.12977930550394</v>
       </c>
       <c r="G24" t="n">
-        <v>0.2110154628753662</v>
+        <v>0.08796191215515137</v>
       </c>
     </row>
     <row r="25">
@@ -1005,22 +1027,22 @@
         <v>24</v>
       </c>
       <c r="B25" t="n">
-        <v>94.02732494954199</v>
+        <v>94.20586865393572</v>
       </c>
       <c r="C25" t="n">
-        <v>96.96711672249108</v>
+        <v>96.94945187820085</v>
       </c>
       <c r="D25" t="n">
-        <v>0.04314804077148438</v>
+        <v>0.02592945098876953</v>
       </c>
       <c r="E25" t="n">
-        <v>92.96679197994987</v>
+        <v>92.79459711224965</v>
       </c>
       <c r="F25" t="n">
-        <v>95.84941520467835</v>
+        <v>95.81366703565877</v>
       </c>
       <c r="G25" t="n">
-        <v>0.1740396022796631</v>
+        <v>0.070526123046875</v>
       </c>
     </row>
     <row r="26">
@@ -1028,22 +1050,22 @@
         <v>25</v>
       </c>
       <c r="B26" t="n">
-        <v>94.19965843813071</v>
+        <v>93.84878124514826</v>
       </c>
       <c r="C26" t="n">
-        <v>96.93488991728219</v>
+        <v>96.42531266027538</v>
       </c>
       <c r="D26" t="n">
-        <v>0.06095123291015625</v>
+        <v>0.02813839912414551</v>
       </c>
       <c r="E26" t="n">
-        <v>93.1484962406015</v>
+        <v>93.32091290172335</v>
       </c>
       <c r="F26" t="n">
-        <v>95.99321278493292</v>
+        <v>95.82875859234167</v>
       </c>
       <c r="G26" t="n">
-        <v>0.2100198268890381</v>
+        <v>0.07810473442077637</v>
       </c>
     </row>
     <row r="27">
@@ -1051,22 +1073,22 @@
         <v>26</v>
       </c>
       <c r="B27" t="n">
-        <v>93.6811054184133</v>
+        <v>93.8441235832945</v>
       </c>
       <c r="C27" t="n">
-        <v>96.27940921690922</v>
+        <v>96.69584100110417</v>
       </c>
       <c r="D27" t="n">
-        <v>0.03316187858581543</v>
+        <v>0.006505727767944336</v>
       </c>
       <c r="E27" t="n">
-        <v>93.32393483709274</v>
+        <v>92.97469337059464</v>
       </c>
       <c r="F27" t="n">
-        <v>96.03413355986886</v>
+        <v>95.84353792185671</v>
       </c>
       <c r="G27" t="n">
-        <v>0.195000171661377</v>
+        <v>0.08644819259643555</v>
       </c>
     </row>
     <row r="28">
@@ -1074,22 +1096,22 @@
         <v>27</v>
       </c>
       <c r="B28" t="n">
-        <v>93.67334264865704</v>
+        <v>94.38130725042694</v>
       </c>
       <c r="C28" t="n">
-        <v>96.67847490347491</v>
+        <v>97.16154252338463</v>
       </c>
       <c r="D28" t="n">
-        <v>0.04587674140930176</v>
+        <v>0.02012252807617188</v>
       </c>
       <c r="E28" t="n">
-        <v>92.60964912280703</v>
+        <v>92.44527247321844</v>
       </c>
       <c r="F28" t="n">
-        <v>96.1910549838754</v>
+        <v>96.27017174385595</v>
       </c>
       <c r="G28" t="n">
-        <v>0.1881477832794189</v>
+        <v>0.0760047435760498</v>
       </c>
     </row>
     <row r="29">
@@ -1097,22 +1119,22 @@
         <v>28</v>
       </c>
       <c r="B29" t="n">
-        <v>93.49479894426331</v>
+        <v>93.49014128240955</v>
       </c>
       <c r="C29" t="n">
-        <v>96.45492957746478</v>
+        <v>96.29160131397229</v>
       </c>
       <c r="D29" t="n">
-        <v>0.0279238224029541</v>
+        <v>0.0312504768371582</v>
       </c>
       <c r="E29" t="n">
-        <v>92.97619047619045</v>
+        <v>92.97624592454588</v>
       </c>
       <c r="F29" t="n">
-        <v>96.15434362176038</v>
+        <v>96.07402542361086</v>
       </c>
       <c r="G29" t="n">
-        <v>0.1950685977935791</v>
+        <v>0.06898951530456543</v>
       </c>
     </row>
     <row r="30">
@@ -1120,22 +1142,22 @@
         <v>29</v>
       </c>
       <c r="B30" t="n">
-        <v>93.85033379909953</v>
+        <v>93.49635149821458</v>
       </c>
       <c r="C30" t="n">
-        <v>96.90893155599039</v>
+        <v>96.3476524663902</v>
       </c>
       <c r="D30" t="n">
-        <v>0.05359387397766113</v>
+        <v>0.03124904632568359</v>
       </c>
       <c r="E30" t="n">
-        <v>93.49937343358394</v>
+        <v>92.97314081664338</v>
       </c>
       <c r="F30" t="n">
-        <v>96.34663234663236</v>
+        <v>95.48981148523484</v>
       </c>
       <c r="G30" t="n">
-        <v>0.1379101276397705</v>
+        <v>0.0846247673034668</v>
       </c>
     </row>
     <row r="31">
@@ -1143,22 +1165,2260 @@
         <v>30</v>
       </c>
       <c r="B31" t="n">
-        <v>93.84722869119703</v>
+        <v>94.02732494954199</v>
       </c>
       <c r="C31" t="n">
-        <v>96.71506583359809</v>
+        <v>97.20895271667797</v>
       </c>
       <c r="D31" t="n">
-        <v>0.05459833145141602</v>
+        <v>0.03124380111694336</v>
       </c>
       <c r="E31" t="n">
+        <v>92.78993945039589</v>
+      </c>
+      <c r="F31" t="n">
+        <v>95.4882903363103</v>
+      </c>
+      <c r="G31" t="n">
+        <v>0.05337071418762207</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G31"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Amostras</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Acurácia Naive Bayes</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Recall Naive Bayes</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Tempo Naive Bayes</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Acurácia Knn</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Recall Knn</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Tempo Knn</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="n">
+        <v>93.8533834586466</v>
+      </c>
+      <c r="C2" t="n">
+        <v>96.83180217365775</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.04683947563171387</v>
+      </c>
+      <c r="E2" t="n">
+        <v>93.15476190476191</v>
+      </c>
+      <c r="F2" t="n">
+        <v>95.68666771948344</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.1093530654907227</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="n">
+        <v>94.02255639097744</v>
+      </c>
+      <c r="C3" t="n">
+        <v>96.76028586077494</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.03776073455810547</v>
+      </c>
+      <c r="E3" t="n">
         <v>93.49937343358394</v>
       </c>
+      <c r="F3" t="n">
+        <v>96.12806111064624</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.1158673763275146</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="n">
+        <v>94.01942355889726</v>
+      </c>
+      <c r="C4" t="n">
+        <v>97.11178629928628</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.03775477409362793</v>
+      </c>
+      <c r="E4" t="n">
+        <v>93.14536340852131</v>
+      </c>
+      <c r="F4" t="n">
+        <v>95.44484195212665</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.1315569877624512</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="n">
+        <v>93.84711779448622</v>
+      </c>
+      <c r="C5" t="n">
+        <v>96.5828156778659</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.06249332427978516</v>
+      </c>
+      <c r="E5" t="n">
+        <v>94.01002506265664</v>
+      </c>
+      <c r="F5" t="n">
+        <v>96.3807283980303</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0.1223850250244141</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="n">
+        <v>93.6779448621554</v>
+      </c>
+      <c r="C6" t="n">
+        <v>96.45358578064125</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.04686474800109863</v>
+      </c>
+      <c r="E6" t="n">
+        <v>92.79135338345866</v>
+      </c>
+      <c r="F6" t="n">
+        <v>95.76350916738292</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0.1158614158630371</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="n">
+        <v>94.02882205513784</v>
+      </c>
+      <c r="C7" t="n">
+        <v>97.22410776994819</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.06416463851928711</v>
+      </c>
+      <c r="E7" t="n">
+        <v>92.96679197994987</v>
+      </c>
+      <c r="F7" t="n">
+        <v>95.77450729095466</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0.1031248569488525</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="n">
+        <v>93.50250626566415</v>
+      </c>
+      <c r="C8" t="n">
+        <v>96.40853693963368</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.05045557022094727</v>
+      </c>
+      <c r="E8" t="n">
+        <v>93.15162907268169</v>
+      </c>
+      <c r="F8" t="n">
+        <v>95.923266124592</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0.1109156608581543</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="n">
+        <v>93.66854636591479</v>
+      </c>
+      <c r="C9" t="n">
+        <v>96.54639687323575</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.06059527397155762</v>
+      </c>
+      <c r="E9" t="n">
+        <v>92.78822055137844</v>
+      </c>
+      <c r="F9" t="n">
+        <v>95.33636788048554</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0.1108994483947754</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="n">
+        <v>93.85964912280701</v>
+      </c>
+      <c r="C10" t="n">
+        <v>96.60596483580355</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.04243040084838867</v>
+      </c>
+      <c r="E10" t="n">
+        <v>93.50250626566414</v>
+      </c>
+      <c r="F10" t="n">
+        <v>96.35200473091719</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0.1099305152893066</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="n">
+        <v>93.85338345864662</v>
+      </c>
+      <c r="C11" t="n">
+        <v>96.31217911459846</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.0367588996887207</v>
+      </c>
+      <c r="E11" t="n">
+        <v>93.32393483709274</v>
+      </c>
+      <c r="F11" t="n">
+        <v>95.6603762384747</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0.1158664226531982</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" t="n">
+        <v>94.02882205513784</v>
+      </c>
+      <c r="C12" t="n">
+        <v>96.67863817229521</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0.06248950958251953</v>
+      </c>
+      <c r="E12" t="n">
+        <v>93.30200501253132</v>
+      </c>
+      <c r="F12" t="n">
+        <v>95.65222993737115</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0.1088569164276123</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" t="n">
+        <v>94.20426065162907</v>
+      </c>
+      <c r="C13" t="n">
+        <v>97.17409389046765</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0.05052852630615234</v>
+      </c>
+      <c r="E13" t="n">
+        <v>93.32080200501254</v>
+      </c>
+      <c r="F13" t="n">
+        <v>95.88259786489527</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0.1162762641906738</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" t="n">
+        <v>94.02255639097744</v>
+      </c>
+      <c r="C14" t="n">
+        <v>96.87533157726847</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0.05256843566894531</v>
+      </c>
+      <c r="E14" t="n">
+        <v>93.8533834586466</v>
+      </c>
+      <c r="F14" t="n">
+        <v>96.46955150443098</v>
+      </c>
+      <c r="G14" t="n">
+        <v>0.1029293537139893</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" t="n">
+        <v>93.8408521303258</v>
+      </c>
+      <c r="C15" t="n">
+        <v>96.62071007264694</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0.0504453182220459</v>
+      </c>
+      <c r="E15" t="n">
+        <v>92.96679197994987</v>
+      </c>
+      <c r="F15" t="n">
+        <v>96.13312309382417</v>
+      </c>
+      <c r="G15" t="n">
+        <v>0.1130986213684082</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" t="n">
+        <v>94.02882205513784</v>
+      </c>
+      <c r="C16" t="n">
+        <v>97.17491526315054</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0.0805351734161377</v>
+      </c>
+      <c r="E16" t="n">
+        <v>92.79761904761902</v>
+      </c>
+      <c r="F16" t="n">
+        <v>95.67622771920439</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0.183690071105957</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" t="n">
+        <v>93.66854636591478</v>
+      </c>
+      <c r="C17" t="n">
+        <v>96.61268677240352</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0.08978104591369629</v>
+      </c>
+      <c r="E17" t="n">
+        <v>92.96992481203009</v>
+      </c>
+      <c r="F17" t="n">
+        <v>95.69251009184663</v>
+      </c>
+      <c r="G17" t="n">
+        <v>0.1513607501983643</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" t="n">
+        <v>93.85651629072683</v>
+      </c>
+      <c r="C18" t="n">
+        <v>96.91475294571269</v>
+      </c>
+      <c r="D18" t="n">
+        <v>0.0462348461151123</v>
+      </c>
+      <c r="E18" t="n">
+        <v>93.32393483709274</v>
+      </c>
+      <c r="F18" t="n">
+        <v>96.05552158493336</v>
+      </c>
+      <c r="G18" t="n">
+        <v>0.1167166233062744</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" t="n">
+        <v>93.85651629072683</v>
+      </c>
+      <c r="C19" t="n">
+        <v>96.88508417920183</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0.05888557434082031</v>
+      </c>
+      <c r="E19" t="n">
+        <v>93.14223057644109</v>
+      </c>
+      <c r="F19" t="n">
+        <v>95.75884438588614</v>
+      </c>
+      <c r="G19" t="n">
+        <v>0.1062080860137939</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" t="n">
+        <v>93.84711779448622</v>
+      </c>
+      <c r="C20" t="n">
+        <v>96.69814618516307</v>
+      </c>
+      <c r="D20" t="n">
+        <v>0.06188797950744629</v>
+      </c>
+      <c r="E20" t="n">
+        <v>92.26817042606517</v>
+      </c>
+      <c r="F20" t="n">
+        <v>95.16058289220052</v>
+      </c>
+      <c r="G20" t="n">
+        <v>0.1069426536560059</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" t="n">
+        <v>94.20426065162906</v>
+      </c>
+      <c r="C21" t="n">
+        <v>97.16719187675069</v>
+      </c>
+      <c r="D21" t="n">
+        <v>0.0584104061126709</v>
+      </c>
+      <c r="E21" t="n">
+        <v>93.32080200501252</v>
+      </c>
+      <c r="F21" t="n">
+        <v>96.34889561669749</v>
+      </c>
+      <c r="G21" t="n">
+        <v>0.1093335151672363</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" t="n">
+        <v>94.20112781954887</v>
+      </c>
+      <c r="C22" t="n">
+        <v>97.01660483696276</v>
+      </c>
+      <c r="D22" t="n">
+        <v>0.06252717971801758</v>
+      </c>
+      <c r="E22" t="n">
+        <v>93.32393483709274</v>
+      </c>
+      <c r="F22" t="n">
+        <v>96.42125156701316</v>
+      </c>
+      <c r="G22" t="n">
+        <v>0.115868091583252</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" t="n">
+        <v>93.85651629072683</v>
+      </c>
+      <c r="C23" t="n">
+        <v>96.35005405671041</v>
+      </c>
+      <c r="D23" t="n">
+        <v>0.05338382720947266</v>
+      </c>
+      <c r="E23" t="n">
+        <v>92.61591478696742</v>
+      </c>
+      <c r="F23" t="n">
+        <v>95.87470766781111</v>
+      </c>
+      <c r="G23" t="n">
+        <v>0.1002829074859619</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" t="n">
+        <v>94.02882205513784</v>
+      </c>
+      <c r="C24" t="n">
+        <v>96.97275903407932</v>
+      </c>
+      <c r="D24" t="n">
+        <v>0.06905150413513184</v>
+      </c>
+      <c r="E24" t="n">
+        <v>93.32393483709274</v>
+      </c>
+      <c r="F24" t="n">
+        <v>96.18008382714265</v>
+      </c>
+      <c r="G24" t="n">
+        <v>0.1022889614105225</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" t="n">
+        <v>93.85651629072682</v>
+      </c>
+      <c r="C25" t="n">
+        <v>97.00722777621691</v>
+      </c>
+      <c r="D25" t="n">
+        <v>0.05735683441162109</v>
+      </c>
+      <c r="E25" t="n">
+        <v>93.32080200501254</v>
+      </c>
+      <c r="F25" t="n">
+        <v>96.03713077188686</v>
+      </c>
+      <c r="G25" t="n">
+        <v>0.1109738349914551</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" t="n">
+        <v>93.84711779448622</v>
+      </c>
+      <c r="C26" t="n">
+        <v>96.80786066312382</v>
+      </c>
+      <c r="D26" t="n">
+        <v>0.05042314529418945</v>
+      </c>
+      <c r="E26" t="n">
+        <v>93.32706766917292</v>
+      </c>
+      <c r="F26" t="n">
+        <v>96.29576012502842</v>
+      </c>
+      <c r="G26" t="n">
+        <v>0.1049563884735107</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" t="n">
+        <v>93.84398496240601</v>
+      </c>
+      <c r="C27" t="n">
+        <v>97.02210463948269</v>
+      </c>
+      <c r="D27" t="n">
+        <v>0.06045198440551758</v>
+      </c>
+      <c r="E27" t="n">
+        <v>93.32706766917292</v>
+      </c>
+      <c r="F27" t="n">
+        <v>96.503087003087</v>
+      </c>
+      <c r="G27" t="n">
+        <v>0.1108996868133545</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" t="n">
+        <v>94.03195488721805</v>
+      </c>
+      <c r="C28" t="n">
+        <v>96.87604012681412</v>
+      </c>
+      <c r="D28" t="n">
+        <v>0.04730129241943359</v>
+      </c>
+      <c r="E28" t="n">
+        <v>93.1359649122807</v>
+      </c>
+      <c r="F28" t="n">
+        <v>95.72101693739069</v>
+      </c>
+      <c r="G28" t="n">
+        <v>0.1158747673034668</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" t="n">
+        <v>94.02568922305765</v>
+      </c>
+      <c r="C29" t="n">
+        <v>96.87140741742259</v>
+      </c>
+      <c r="D29" t="n">
+        <v>0.06248831748962402</v>
+      </c>
+      <c r="E29" t="n">
+        <v>92.97305764411027</v>
+      </c>
+      <c r="F29" t="n">
+        <v>96.02952532364297</v>
+      </c>
+      <c r="G29" t="n">
+        <v>0.1002485752105713</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" t="n">
+        <v>93.84398496240604</v>
+      </c>
+      <c r="C30" t="n">
+        <v>96.64886368112174</v>
+      </c>
+      <c r="D30" t="n">
+        <v>0.05648469924926758</v>
+      </c>
+      <c r="E30" t="n">
+        <v>93.32393483709274</v>
+      </c>
+      <c r="F30" t="n">
+        <v>96.4567597153804</v>
+      </c>
+      <c r="G30" t="n">
+        <v>0.1111080646514893</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" t="n">
+        <v>93.50563909774436</v>
+      </c>
+      <c r="C31" t="n">
+        <v>96.41398390764093</v>
+      </c>
+      <c r="D31" t="n">
+        <v>0.05852580070495605</v>
+      </c>
+      <c r="E31" t="n">
+        <v>93.30827067669173</v>
+      </c>
       <c r="F31" t="n">
-        <v>96.07123170514016</v>
+        <v>95.58069718142313</v>
       </c>
       <c r="G31" t="n">
-        <v>0.1711251735687256</v>
+        <v>0.09786772727966309</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G31"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Amostras</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Acurácia Naive Bayes</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Recall Naive Bayes</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Tempo Naive Bayes</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Acurácia Knn</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Recall Knn</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Tempo Knn</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="n">
+        <v>96.19364534134822</v>
+      </c>
+      <c r="C2" t="n">
+        <v>97.58714328033967</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.03124356269836426</v>
+      </c>
+      <c r="E2" t="n">
+        <v>96.92464577071705</v>
+      </c>
+      <c r="F2" t="n">
+        <v>95.44284415348244</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.08461904525756836</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="n">
+        <v>96.34392443108631</v>
+      </c>
+      <c r="C3" t="n">
+        <v>97.82967032967032</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.03775477409362793</v>
+      </c>
+      <c r="E3" t="n">
+        <v>97.06955775010735</v>
+      </c>
+      <c r="F3" t="n">
+        <v>96.26821705426357</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.07815384864807129</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="n">
+        <v>96.33963074280807</v>
+      </c>
+      <c r="C4" t="n">
+        <v>97.83333333333333</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.03772687911987305</v>
+      </c>
+      <c r="E4" t="n">
+        <v>97.36474881923571</v>
+      </c>
+      <c r="F4" t="n">
+        <v>96.69224211423699</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.08461380004882812</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="n">
+        <v>95.90167453842851</v>
+      </c>
+      <c r="C5" t="n">
+        <v>96.92994318195348</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.03125143051147461</v>
+      </c>
+      <c r="E5" t="n">
+        <v>97.07170459424646</v>
+      </c>
+      <c r="F5" t="n">
+        <v>95.98464978490495</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0.0790867805480957</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="n">
+        <v>96.19364534134822</v>
+      </c>
+      <c r="C6" t="n">
+        <v>97.4641771602258</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.0156254768371582</v>
+      </c>
+      <c r="E6" t="n">
+        <v>97.06955775010735</v>
+      </c>
+      <c r="F6" t="n">
+        <v>96.17180663002765</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0.09013772010803223</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="n">
+        <v>96.04658651781881</v>
+      </c>
+      <c r="C7" t="n">
+        <v>97.44873209158924</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.03125119209289551</v>
+      </c>
+      <c r="E7" t="n">
+        <v>97.3658222413053</v>
+      </c>
+      <c r="F7" t="n">
+        <v>97.07949055775143</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0.08458542823791504</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="n">
+        <v>96.34070416487764</v>
+      </c>
+      <c r="C8" t="n">
+        <v>97.98726467331119</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.03124117851257324</v>
+      </c>
+      <c r="E8" t="n">
+        <v>97.80270502361527</v>
+      </c>
+      <c r="F8" t="n">
+        <v>97.48566334746458</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0.08462190628051758</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="n">
+        <v>96.19793902962644</v>
+      </c>
+      <c r="C9" t="n">
+        <v>97.71320754716982</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.03130316734313965</v>
+      </c>
+      <c r="E9" t="n">
+        <v>97.80163160154572</v>
+      </c>
+      <c r="F9" t="n">
+        <v>97.43451536643025</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0.0690007209777832</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="n">
+        <v>96.34070416487764</v>
+      </c>
+      <c r="C10" t="n">
+        <v>97.65031626685762</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.02212810516357422</v>
+      </c>
+      <c r="E10" t="n">
+        <v>97.65671962215544</v>
+      </c>
+      <c r="F10" t="n">
+        <v>97.13499209398734</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0.07355451583862305</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="n">
+        <v>95.7546157148991</v>
+      </c>
+      <c r="C11" t="n">
+        <v>97.11458394850293</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.02664446830749512</v>
+      </c>
+      <c r="E11" t="n">
+        <v>97.80592528982396</v>
+      </c>
+      <c r="F11" t="n">
+        <v>97.4190564292322</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0.1314799785614014</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" t="n">
+        <v>96.04658651781881</v>
+      </c>
+      <c r="C12" t="n">
+        <v>96.96132299073476</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0.04686594009399414</v>
+      </c>
+      <c r="E12" t="n">
+        <v>97.21983683984543</v>
+      </c>
+      <c r="F12" t="n">
+        <v>96.42645932350329</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0.1158716678619385</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" t="n">
+        <v>96.04443967367968</v>
+      </c>
+      <c r="C13" t="n">
+        <v>97.48187549251381</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0.07503437995910645</v>
+      </c>
+      <c r="E13" t="n">
+        <v>97.21661657363676</v>
+      </c>
+      <c r="F13" t="n">
+        <v>95.84603350578961</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0.1067972183227539</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" t="n">
+        <v>95.60541004723056</v>
+      </c>
+      <c r="C14" t="n">
+        <v>97.27856790685327</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0.0381920337677002</v>
+      </c>
+      <c r="E14" t="n">
+        <v>96.92249892657794</v>
+      </c>
+      <c r="F14" t="n">
+        <v>95.29911358482786</v>
+      </c>
+      <c r="G14" t="n">
+        <v>0.07652401924133301</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" t="n">
+        <v>96.19364534134822</v>
+      </c>
+      <c r="C15" t="n">
+        <v>98.02962962962964</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0.01562070846557617</v>
+      </c>
+      <c r="E15" t="n">
+        <v>97.07492486045514</v>
+      </c>
+      <c r="F15" t="n">
+        <v>96.35028378585673</v>
+      </c>
+      <c r="G15" t="n">
+        <v>0.1002433300018311</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" t="n">
+        <v>96.19471876341777</v>
+      </c>
+      <c r="C16" t="n">
+        <v>97.4985507246377</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0.01562094688415527</v>
+      </c>
+      <c r="E16" t="n">
+        <v>97.21876341777588</v>
+      </c>
+      <c r="F16" t="n">
+        <v>97.13619210977701</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0.09376120567321777</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" t="n">
+        <v>96.19149849720911</v>
+      </c>
+      <c r="C17" t="n">
+        <v>97.45297977581873</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0.02759766578674316</v>
+      </c>
+      <c r="E17" t="n">
+        <v>96.92249892657794</v>
+      </c>
+      <c r="F17" t="n">
+        <v>96.0139353400223</v>
+      </c>
+      <c r="G17" t="n">
+        <v>0.08682537078857422</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" t="n">
+        <v>96.19257191927866</v>
+      </c>
+      <c r="C18" t="n">
+        <v>97.49372725834519</v>
+      </c>
+      <c r="D18" t="n">
+        <v>0.01312375068664551</v>
+      </c>
+      <c r="E18" t="n">
+        <v>97.50751395448691</v>
+      </c>
+      <c r="F18" t="n">
+        <v>96.65146745146747</v>
+      </c>
+      <c r="G18" t="n">
+        <v>0.08461523056030273</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" t="n">
+        <v>96.05088020609705</v>
+      </c>
+      <c r="C19" t="n">
+        <v>97.44107744107744</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0.01562929153442383</v>
+      </c>
+      <c r="E19" t="n">
+        <v>97.07492486045514</v>
+      </c>
+      <c r="F19" t="n">
+        <v>96.09764309764309</v>
+      </c>
+      <c r="G19" t="n">
+        <v>0.09475851058959961</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" t="n">
+        <v>96.04873336195793</v>
+      </c>
+      <c r="C20" t="n">
+        <v>97.21407837445574</v>
+      </c>
+      <c r="D20" t="n">
+        <v>0.03021597862243652</v>
+      </c>
+      <c r="E20" t="n">
+        <v>97.36367539716618</v>
+      </c>
+      <c r="F20" t="n">
+        <v>96.80758422629158</v>
+      </c>
+      <c r="G20" t="n">
+        <v>0.07468128204345703</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" t="n">
+        <v>96.19257191927866</v>
+      </c>
+      <c r="C21" t="n">
+        <v>97.91162887455795</v>
+      </c>
+      <c r="D21" t="n">
+        <v>0.03026700019836426</v>
+      </c>
+      <c r="E21" t="n">
+        <v>96.92142550450838</v>
+      </c>
+      <c r="F21" t="n">
+        <v>96.03823620104841</v>
+      </c>
+      <c r="G21" t="n">
+        <v>0.08072590827941895</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" t="n">
+        <v>96.20008587376556</v>
+      </c>
+      <c r="C22" t="n">
+        <v>97.85555555555557</v>
+      </c>
+      <c r="D22" t="n">
+        <v>0.03021812438964844</v>
+      </c>
+      <c r="E22" t="n">
+        <v>97.36367539716616</v>
+      </c>
+      <c r="F22" t="n">
+        <v>96.83783471109149</v>
+      </c>
+      <c r="G22" t="n">
+        <v>0.09095549583435059</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" t="n">
+        <v>96.19042507513956</v>
+      </c>
+      <c r="C23" t="n">
+        <v>97.50184840734713</v>
+      </c>
+      <c r="D23" t="n">
+        <v>0.02016544342041016</v>
+      </c>
+      <c r="E23" t="n">
+        <v>97.50966079862602</v>
+      </c>
+      <c r="F23" t="n">
+        <v>97.52774464983767</v>
+      </c>
+      <c r="G23" t="n">
+        <v>0.0806126594543457</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" t="n">
+        <v>96.19364534134822</v>
+      </c>
+      <c r="C24" t="n">
+        <v>97.43400588482555</v>
+      </c>
+      <c r="D24" t="n">
+        <v>0.02819705009460449</v>
+      </c>
+      <c r="E24" t="n">
+        <v>97.50858737655645</v>
+      </c>
+      <c r="F24" t="n">
+        <v>96.68743983381466</v>
+      </c>
+      <c r="G24" t="n">
+        <v>0.09081506729125977</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" t="n">
+        <v>96.34177758694719</v>
+      </c>
+      <c r="C25" t="n">
+        <v>97.88458225667527</v>
+      </c>
+      <c r="D25" t="n">
+        <v>0.02219486236572266</v>
+      </c>
+      <c r="E25" t="n">
+        <v>97.22198368398456</v>
+      </c>
+      <c r="F25" t="n">
+        <v>95.46385809312639</v>
+      </c>
+      <c r="G25" t="n">
+        <v>0.07855081558227539</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" t="n">
+        <v>96.49098325461573</v>
+      </c>
+      <c r="C26" t="n">
+        <v>98.34707216219823</v>
+      </c>
+      <c r="D26" t="n">
+        <v>0.03225231170654297</v>
+      </c>
+      <c r="E26" t="n">
+        <v>96.9257191927866</v>
+      </c>
+      <c r="F26" t="n">
+        <v>95.84223602484471</v>
+      </c>
+      <c r="G26" t="n">
+        <v>0.08058714866638184</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" t="n">
+        <v>96.19364534134822</v>
+      </c>
+      <c r="C27" t="n">
+        <v>97.44768839837676</v>
+      </c>
+      <c r="D27" t="n">
+        <v>0.02698445320129395</v>
+      </c>
+      <c r="E27" t="n">
+        <v>96.7786603692572</v>
+      </c>
+      <c r="F27" t="n">
+        <v>95.33431480799901</v>
+      </c>
+      <c r="G27" t="n">
+        <v>0.07478499412536621</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" t="n">
+        <v>96.33641047659941</v>
+      </c>
+      <c r="C28" t="n">
+        <v>97.84090909090909</v>
+      </c>
+      <c r="D28" t="n">
+        <v>0.03775596618652344</v>
+      </c>
+      <c r="E28" t="n">
+        <v>96.92679261485615</v>
+      </c>
+      <c r="F28" t="n">
+        <v>95.94472161300945</v>
+      </c>
+      <c r="G28" t="n">
+        <v>0.07811379432678223</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" t="n">
+        <v>96.34070416487764</v>
+      </c>
+      <c r="C29" t="n">
+        <v>97.8080637132902</v>
+      </c>
+      <c r="D29" t="n">
+        <v>0.02212882041931152</v>
+      </c>
+      <c r="E29" t="n">
+        <v>97.07385143838557</v>
+      </c>
+      <c r="F29" t="n">
+        <v>95.82414480748582</v>
+      </c>
+      <c r="G29" t="n">
+        <v>0.0937349796295166</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" t="n">
+        <v>96.19042507513956</v>
+      </c>
+      <c r="C30" t="n">
+        <v>97.6900284900285</v>
+      </c>
+      <c r="D30" t="n">
+        <v>0.02213740348815918</v>
+      </c>
+      <c r="E30" t="n">
+        <v>97.07277801631602</v>
+      </c>
+      <c r="F30" t="n">
+        <v>95.84209092035178</v>
+      </c>
+      <c r="G30" t="n">
+        <v>0.08461809158325195</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" t="n">
+        <v>96.33748389866896</v>
+      </c>
+      <c r="C31" t="n">
+        <v>97.89439071566733</v>
+      </c>
+      <c r="D31" t="n">
+        <v>0.03125333786010742</v>
+      </c>
+      <c r="E31" t="n">
+        <v>97.95298411335338</v>
+      </c>
+      <c r="F31" t="n">
+        <v>97.90162701668035</v>
+      </c>
+      <c r="G31" t="n">
+        <v>0.08342933654785156</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G31"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Amostras</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Acurácia Naive Bayes</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Recall Naive Bayes</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Tempo Naive Bayes</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Acurácia Knn</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Recall Knn</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Tempo Knn</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="n">
+        <v>96.19991474850809</v>
+      </c>
+      <c r="C2" t="n">
+        <v>97.41074714758925</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.07449483871459961</v>
+      </c>
+      <c r="E2" t="n">
+        <v>97.65984654731457</v>
+      </c>
+      <c r="F2" t="n">
+        <v>97.55037972779907</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.2397425174713135</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="n">
+        <v>96.33631713554986</v>
+      </c>
+      <c r="C3" t="n">
+        <v>97.97978830133806</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.05784821510314941</v>
+      </c>
+      <c r="E3" t="n">
+        <v>97.65345268542201</v>
+      </c>
+      <c r="F3" t="n">
+        <v>97.28549388900018</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.1326782703399658</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="n">
+        <v>96.33844842284741</v>
+      </c>
+      <c r="C4" t="n">
+        <v>98.05093167701864</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.09973049163818359</v>
+      </c>
+      <c r="E4" t="n">
+        <v>97.36359761295823</v>
+      </c>
+      <c r="F4" t="n">
+        <v>96.51471861471862</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.1413760185241699</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="n">
+        <v>96.04859335038365</v>
+      </c>
+      <c r="C5" t="n">
+        <v>96.9352472089314</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.0465855598449707</v>
+      </c>
+      <c r="E5" t="n">
+        <v>97.36359761295823</v>
+      </c>
+      <c r="F5" t="n">
+        <v>96.8937728937729</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0.1129579544067383</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="n">
+        <v>96.34057971014492</v>
+      </c>
+      <c r="C6" t="n">
+        <v>98.03649237472767</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.06085395812988281</v>
+      </c>
+      <c r="E6" t="n">
+        <v>97.21440750213128</v>
+      </c>
+      <c r="F6" t="n">
+        <v>97.31878306878308</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0.1147201061248779</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="n">
+        <v>95.90579710144928</v>
+      </c>
+      <c r="C7" t="n">
+        <v>97.1207729468599</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.08083558082580566</v>
+      </c>
+      <c r="E7" t="n">
+        <v>97.37212276214834</v>
+      </c>
+      <c r="F7" t="n">
+        <v>96.41358496575889</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0.1266567707061768</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="n">
+        <v>96.05072463768116</v>
+      </c>
+      <c r="C8" t="n">
+        <v>97.1075454336324</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.05784416198730469</v>
+      </c>
+      <c r="E8" t="n">
+        <v>97.21867007672633</v>
+      </c>
+      <c r="F8" t="n">
+        <v>96.91711569428961</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0.1196796894073486</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="n">
+        <v>96.33205456095482</v>
+      </c>
+      <c r="C9" t="n">
+        <v>97.49282296650718</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.07280540466308594</v>
+      </c>
+      <c r="E9" t="n">
+        <v>97.35933503836318</v>
+      </c>
+      <c r="F9" t="n">
+        <v>96.68352356178444</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0.2082417011260986</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="n">
+        <v>96.18712702472294</v>
+      </c>
+      <c r="C10" t="n">
+        <v>98.02834757834759</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.0957329273223877</v>
+      </c>
+      <c r="E10" t="n">
+        <v>97.21653878942881</v>
+      </c>
+      <c r="F10" t="n">
+        <v>96.48354978354978</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0.1881122589111328</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="n">
+        <v>96.19138959931799</v>
+      </c>
+      <c r="C11" t="n">
+        <v>97.94307359307359</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.04892110824584961</v>
+      </c>
+      <c r="E11" t="n">
+        <v>97.36786018755328</v>
+      </c>
+      <c r="F11" t="n">
+        <v>96.84577869795261</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0.09474635124206543</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" t="n">
+        <v>96.48124467178174</v>
+      </c>
+      <c r="C12" t="n">
+        <v>98.14743589743588</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0.04687333106994629</v>
+      </c>
+      <c r="E12" t="n">
+        <v>97.21227621483376</v>
+      </c>
+      <c r="F12" t="n">
+        <v>96.35411255411256</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0.1176786422729492</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" t="n">
+        <v>96.33844842284741</v>
+      </c>
+      <c r="C13" t="n">
+        <v>97.74824600686669</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0.04690074920654297</v>
+      </c>
+      <c r="E13" t="n">
+        <v>97.21867007672633</v>
+      </c>
+      <c r="F13" t="n">
+        <v>96.14607244607244</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0.1162757873535156</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" t="n">
+        <v>96.19352088661553</v>
+      </c>
+      <c r="C14" t="n">
+        <v>97.90665855883248</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0.04962897300720215</v>
+      </c>
+      <c r="E14" t="n">
+        <v>97.65558397271953</v>
+      </c>
+      <c r="F14" t="n">
+        <v>96.62632850241548</v>
+      </c>
+      <c r="G14" t="n">
+        <v>0.1022593975067139</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" t="n">
+        <v>96.34484228473997</v>
+      </c>
+      <c r="C15" t="n">
+        <v>97.94144116752811</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0.06249618530273438</v>
+      </c>
+      <c r="E15" t="n">
+        <v>97.65771526001706</v>
+      </c>
+      <c r="F15" t="n">
+        <v>96.98365914445374</v>
+      </c>
+      <c r="G15" t="n">
+        <v>0.1158692836761475</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" t="n">
+        <v>96.05072463768116</v>
+      </c>
+      <c r="C16" t="n">
+        <v>97.61199819670585</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0.05338311195373535</v>
+      </c>
+      <c r="E16" t="n">
+        <v>97.51705029838021</v>
+      </c>
+      <c r="F16" t="n">
+        <v>97.84033259867761</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0.1171729564666748</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" t="n">
+        <v>95.90153452685422</v>
+      </c>
+      <c r="C17" t="n">
+        <v>96.92750582750583</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0.04937624931335449</v>
+      </c>
+      <c r="E17" t="n">
+        <v>97.6619778346121</v>
+      </c>
+      <c r="F17" t="n">
+        <v>97.11410369019065</v>
+      </c>
+      <c r="G17" t="n">
+        <v>0.1158790588378906</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" t="n">
+        <v>96.19138959931799</v>
+      </c>
+      <c r="C18" t="n">
+        <v>97.63306138306137</v>
+      </c>
+      <c r="D18" t="n">
+        <v>0.04686641693115234</v>
+      </c>
+      <c r="E18" t="n">
+        <v>97.51278772378515</v>
+      </c>
+      <c r="F18" t="n">
+        <v>97.49424123970402</v>
+      </c>
+      <c r="G18" t="n">
+        <v>0.1158707141876221</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" t="n">
+        <v>96.1935208866155</v>
+      </c>
+      <c r="C19" t="n">
+        <v>97.65282422891119</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0.05338263511657715</v>
+      </c>
+      <c r="E19" t="n">
+        <v>97.21440750213131</v>
+      </c>
+      <c r="F19" t="n">
+        <v>96.71120401337794</v>
+      </c>
+      <c r="G19" t="n">
+        <v>0.1158735752105713</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" t="n">
+        <v>96.20204603580562</v>
+      </c>
+      <c r="C20" t="n">
+        <v>98.02834757834758</v>
+      </c>
+      <c r="D20" t="n">
+        <v>0.05074381828308105</v>
+      </c>
+      <c r="E20" t="n">
+        <v>97.07587382779199</v>
+      </c>
+      <c r="F20" t="n">
+        <v>96.20119003803215</v>
+      </c>
+      <c r="G20" t="n">
+        <v>0.1159071922302246</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" t="n">
+        <v>96.05072463768116</v>
+      </c>
+      <c r="C21" t="n">
+        <v>97.17355889724311</v>
+      </c>
+      <c r="D21" t="n">
+        <v>0.06300210952758789</v>
+      </c>
+      <c r="E21" t="n">
+        <v>97.21653878942882</v>
+      </c>
+      <c r="F21" t="n">
+        <v>96.76015076877145</v>
+      </c>
+      <c r="G21" t="n">
+        <v>0.1062521934509277</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" t="n">
+        <v>96.19138959931799</v>
+      </c>
+      <c r="C22" t="n">
+        <v>97.18297258297257</v>
+      </c>
+      <c r="D22" t="n">
+        <v>0.04686832427978516</v>
+      </c>
+      <c r="E22" t="n">
+        <v>96.62830349531119</v>
+      </c>
+      <c r="F22" t="n">
+        <v>95.67196917414307</v>
+      </c>
+      <c r="G22" t="n">
+        <v>0.1158750057220459</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" t="n">
+        <v>96.19138959931799</v>
+      </c>
+      <c r="C23" t="n">
+        <v>97.65216055566685</v>
+      </c>
+      <c r="D23" t="n">
+        <v>0.05165386199951172</v>
+      </c>
+      <c r="E23" t="n">
+        <v>97.21440750213128</v>
+      </c>
+      <c r="F23" t="n">
+        <v>96.33099658961729</v>
+      </c>
+      <c r="G23" t="n">
+        <v>0.1099646091461182</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" t="n">
+        <v>96.1935208866155</v>
+      </c>
+      <c r="C24" t="n">
+        <v>97.30820758189181</v>
+      </c>
+      <c r="D24" t="n">
+        <v>0.0342869758605957</v>
+      </c>
+      <c r="E24" t="n">
+        <v>97.36572890025576</v>
+      </c>
+      <c r="F24" t="n">
+        <v>96.67522770971047</v>
+      </c>
+      <c r="G24" t="n">
+        <v>0.1191492080688477</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" t="n">
+        <v>96.34484228473997</v>
+      </c>
+      <c r="C25" t="n">
+        <v>97.8846486846487</v>
+      </c>
+      <c r="D25" t="n">
+        <v>0.05049252510070801</v>
+      </c>
+      <c r="E25" t="n">
+        <v>97.21867007672633</v>
+      </c>
+      <c r="F25" t="n">
+        <v>96.31621896621898</v>
+      </c>
+      <c r="G25" t="n">
+        <v>0.1219542026519775</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" t="n">
+        <v>96.34057971014492</v>
+      </c>
+      <c r="C26" t="n">
+        <v>97.84391534391534</v>
+      </c>
+      <c r="D26" t="n">
+        <v>0.05425286293029785</v>
+      </c>
+      <c r="E26" t="n">
+        <v>97.36359761295823</v>
+      </c>
+      <c r="F26" t="n">
+        <v>97.52787068004459</v>
+      </c>
+      <c r="G26" t="n">
+        <v>0.1140823364257812</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" t="n">
+        <v>96.33418584825235</v>
+      </c>
+      <c r="C27" t="n">
+        <v>97.93722369584439</v>
+      </c>
+      <c r="D27" t="n">
+        <v>0.04690170288085938</v>
+      </c>
+      <c r="E27" t="n">
+        <v>97.5149190110827</v>
+      </c>
+      <c r="F27" t="n">
+        <v>96.73460798460798</v>
+      </c>
+      <c r="G27" t="n">
+        <v>0.115837574005127</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" t="n">
+        <v>96.04219948849104</v>
+      </c>
+      <c r="C28" t="n">
+        <v>97.13434343434344</v>
+      </c>
+      <c r="D28" t="n">
+        <v>0.05338549613952637</v>
+      </c>
+      <c r="E28" t="n">
+        <v>97.80264279624893</v>
+      </c>
+      <c r="F28" t="n">
+        <v>97.30915792103949</v>
+      </c>
+      <c r="G28" t="n">
+        <v>0.115856409072876</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" t="n">
+        <v>96.19991474850809</v>
+      </c>
+      <c r="C29" t="n">
+        <v>97.43079937304074</v>
+      </c>
+      <c r="D29" t="n">
+        <v>0.03124237060546875</v>
+      </c>
+      <c r="E29" t="n">
+        <v>97.36359761295823</v>
+      </c>
+      <c r="F29" t="n">
+        <v>96.80569358178053</v>
+      </c>
+      <c r="G29" t="n">
+        <v>0.1054079532623291</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" t="n">
+        <v>96.33844842284741</v>
+      </c>
+      <c r="C30" t="n">
+        <v>97.7024720893142</v>
+      </c>
+      <c r="D30" t="n">
+        <v>0.06249356269836426</v>
+      </c>
+      <c r="E30" t="n">
+        <v>97.07800511508951</v>
+      </c>
+      <c r="F30" t="n">
+        <v>96.31913014521709</v>
+      </c>
+      <c r="G30" t="n">
+        <v>0.1158604621887207</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" t="n">
+        <v>96.18925831202047</v>
+      </c>
+      <c r="C31" t="n">
+        <v>97.31969696969698</v>
+      </c>
+      <c r="D31" t="n">
+        <v>0.03669381141662598</v>
+      </c>
+      <c r="E31" t="n">
+        <v>97.21227621483376</v>
+      </c>
+      <c r="F31" t="n">
+        <v>96.03125763125763</v>
+      </c>
+      <c r="G31" t="n">
+        <v>0.1050403118133545</v>
       </c>
     </row>
   </sheetData>

</xml_diff>